<commit_message>
finished preprocessing almost all tables
</commit_message>
<xml_diff>
--- a/Hands On 3 Studi Kasus/HARGA PANGAN DI PASAR ASTAMBUL 2017.xlsx
+++ b/Hands On 3 Studi Kasus/HARGA PANGAN DI PASAR ASTAMBUL 2017.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Kuliah\semester6\KD\Studi Kasus KDD Genap 2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Kuliah\semester6\KD\Data-Mining\Hands On 3 Studi Kasus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC24B85B-8A3C-4369-ADE5-A62FD02EA4C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B66743-0677-4E71-B8D1-E9CA563BCFDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-3720" windowWidth="23256" windowHeight="13176" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="MARET " sheetId="1" r:id="rId1"/>
+    <sheet name="MARET" sheetId="1" r:id="rId1"/>
     <sheet name="APRIL" sheetId="7" r:id="rId2"/>
     <sheet name="MEI" sheetId="8" r:id="rId3"/>
     <sheet name="JUNI" sheetId="9" r:id="rId4"/>
@@ -1080,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1351,7 +1351,10 @@
       </c>
       <c r="I13" s="41"/>
       <c r="J13" s="41"/>
-      <c r="K13" s="22"/>
+      <c r="K13" s="20">
+        <f>AVERAGE(E13:J13)</f>
+        <v>10000</v>
+      </c>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
@@ -2050,8 +2053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="B1:Q52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3020,7 +3023,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="B1:X49"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
@@ -4083,8 +4086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:Q52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5057,7 +5060,7 @@
   <dimension ref="B1:Q52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6067,8 +6070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:Q52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9997,8 +10000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B1:Q52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P7" sqref="O7:P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10970,7 +10973,7 @@
   <dimension ref="B1:Q52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>